<commit_message>
Add support for vertical headers in xlsx extractor
</commit_message>
<xml_diff>
--- a/plugins/xlsx-extractor/ref/test-basic.xlsx
+++ b/plugins/xlsx-extractor/ref/test-basic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carl/FlatFilers/flatfile-plugins/plugins/xlsx-extractor/ref/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/josias/code/flatfile-plugins/plugins/xlsx-extractor/ref/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DAC28DC-2A3E-2944-A3B6-8A55DA6266AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8147C67A-FFE0-7C47-8139-40159F08A29F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1900" windowWidth="27240" windowHeight="16440" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
+    <workbookView xWindow="3000" yWindow="1900" windowWidth="27240" windowHeight="16440" activeTab="2" xr2:uid="{04CC5A6A-75D3-A249-AF92-C18D3CDE3404}"/>
   </bookViews>
   <sheets>
     <sheet name="Departments" sheetId="1" r:id="rId1"/>
@@ -1122,7 +1122,7 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
@@ -4331,7 +4331,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3683B01-89F2-9C47-81C6-DA2BCD151184}">
   <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>